<commit_message>
Made cool graphs for population ecology assignment.
</commit_message>
<xml_diff>
--- a/Data/Other/popecolab11.xlsx
+++ b/Data/Other/popecolab11.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RyanMeyer/Documents/R Projects/Data_Analysis_2022/Data/Other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1832A02E-F30D-254D-B0D4-477BC2842943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6282DE09-0702-7042-A753-FD2BCDA007FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{C45E152F-4FE1-44E0-A414-158CAD2532A4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15660" xr2:uid="{C45E152F-4FE1-44E0-A414-158CAD2532A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="24">
   <si>
     <t>stable distribution</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>90% reduction in F</t>
-  </si>
-  <si>
-    <t>all age classes</t>
   </si>
   <si>
     <t>Young Infection</t>
@@ -93,15 +90,37 @@
   <si>
     <t>reproductive_value</t>
   </si>
+  <si>
+    <t>All Age Class F Reduction</t>
+  </si>
+  <si>
+    <t>model_2</t>
+  </si>
+  <si>
+    <t>model_3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,8 +146,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -195,15 +215,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>352424</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2728</xdr:rowOff>
+      <xdr:colOff>30039</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>168804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>334511</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>105359</xdr:rowOff>
+      <xdr:colOff>12126</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76051</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -226,8 +246,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5962649" y="383728"/>
-          <a:ext cx="2420487" cy="1245631"/>
+          <a:off x="6985731" y="754958"/>
+          <a:ext cx="2678395" cy="1274939"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -370,16 +390,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>604961</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>526806</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>49447</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>170324</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>177880</xdr:rowOff>
+      <xdr:colOff>420076</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>21572</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -402,8 +422,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6883841" y="2217420"/>
-          <a:ext cx="784563" cy="520779"/>
+          <a:off x="7482498" y="2003293"/>
+          <a:ext cx="1915501" cy="1144433"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -414,16 +434,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>434340</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>138014</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>180340</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>43071</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>334443</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>155018</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>488462</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>125711</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -446,8 +466,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6713220" y="2698334"/>
-          <a:ext cx="1119303" cy="748525"/>
+          <a:off x="7136032" y="3364609"/>
+          <a:ext cx="1656276" cy="1059564"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -678,16 +698,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>159130</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>308220</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>149361</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>277354</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>573</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>414124</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>186189</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -710,8 +730,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5762625" y="5493130"/>
-          <a:ext cx="1934704" cy="984443"/>
+          <a:off x="5915758" y="5620130"/>
+          <a:ext cx="2128135" cy="1013751"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -810,16 +830,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>143778</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>378239</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>174381</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>20193</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>729</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>254654</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>117960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -842,8 +862,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6954153" y="5391150"/>
-          <a:ext cx="1705215" cy="1086579"/>
+          <a:off x="9356162" y="6035919"/>
+          <a:ext cx="1898646" cy="1115887"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1152,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F2A1A3-23C7-4825-9E9D-140FB9B7C46E}">
-  <dimension ref="B2:U39"/>
+  <dimension ref="B2:AB99"/>
   <sheetViews>
-    <sheetView topLeftCell="E9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19:T39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19:T99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1167,7 +1187,7 @@
   <sheetData>
     <row r="2" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.2">
@@ -1265,7 +1285,7 @@
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
@@ -1316,16 +1336,16 @@
         <v>0.05</v>
       </c>
       <c r="R16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S16" t="s">
+        <v>12</v>
+      </c>
+      <c r="T16" t="s">
         <v>13</v>
       </c>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>14</v>
-      </c>
-      <c r="U16" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.2">
@@ -1373,13 +1393,13 @@
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.2">
       <c r="Q19" t="s">
+        <v>15</v>
+      </c>
+      <c r="R19" t="s">
         <v>16</v>
       </c>
-      <c r="R19" t="s">
+      <c r="S19" t="s">
         <v>17</v>
-      </c>
-      <c r="S19" t="s">
-        <v>18</v>
       </c>
       <c r="T19" t="s">
         <v>3</v>
@@ -1387,7 +1407,7 @@
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.2">
       <c r="Q20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R20" t="s">
         <v>5</v>
@@ -1401,10 +1421,10 @@
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R21" t="s">
         <v>5</v>
@@ -1418,7 +1438,7 @@
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.2">
       <c r="Q22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R22" t="s">
         <v>5</v>
@@ -1438,7 +1458,7 @@
         <v>1.31</v>
       </c>
       <c r="Q23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R23" t="s">
         <v>5</v>
@@ -1470,7 +1490,7 @@
         <v>5</v>
       </c>
       <c r="Q24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R24" t="s">
         <v>5</v>
@@ -1502,10 +1522,10 @@
         <v>0.03</v>
       </c>
       <c r="Q25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S25">
         <v>0.6</v>
@@ -1534,10 +1554,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="Q26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S26">
         <v>0.2</v>
@@ -1566,10 +1586,10 @@
         <v>0.48</v>
       </c>
       <c r="Q27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S27">
         <v>0.1</v>
@@ -1580,10 +1600,10 @@
     </row>
     <row r="28" spans="2:20" x14ac:dyDescent="0.2">
       <c r="Q28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S28">
         <v>0.06</v>
@@ -1594,10 +1614,10 @@
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.2">
       <c r="Q29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S29">
         <v>0.03</v>
@@ -1611,10 +1631,10 @@
         <v>7</v>
       </c>
       <c r="Q30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S30">
         <v>21.3</v>
@@ -1625,10 +1645,10 @@
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.2">
       <c r="Q31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S31">
         <v>7.3</v>
@@ -1639,16 +1659,16 @@
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
       </c>
       <c r="Q32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S32">
         <v>4</v>
@@ -1665,10 +1685,10 @@
         <v>0.623</v>
       </c>
       <c r="Q33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S33">
         <v>2.1</v>
@@ -1697,10 +1717,10 @@
         <v>5</v>
       </c>
       <c r="Q34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="S34">
         <v>1.1000000000000001</v>
@@ -1729,10 +1749,10 @@
         <v>0.26</v>
       </c>
       <c r="Q35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S35">
         <v>1</v>
@@ -1761,10 +1781,10 @@
         <v>6.7</v>
       </c>
       <c r="Q36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S36">
         <v>1.7</v>
@@ -1793,10 +1813,10 @@
         <v>0.21</v>
       </c>
       <c r="Q37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S37">
         <v>1.8</v>
@@ -1807,10 +1827,10 @@
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.2">
       <c r="Q38" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S38">
         <v>1.5</v>
@@ -1821,10 +1841,10 @@
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.2">
       <c r="Q39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="S39">
         <v>0.96</v>
@@ -1833,7 +1853,932 @@
         <v>5</v>
       </c>
     </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="Q40" t="s">
+        <v>12</v>
+      </c>
+      <c r="R40" t="s">
+        <v>5</v>
+      </c>
+      <c r="S40">
+        <v>0.99</v>
+      </c>
+      <c r="T40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="Q41" t="s">
+        <v>12</v>
+      </c>
+      <c r="R41" t="s">
+        <v>5</v>
+      </c>
+      <c r="S41">
+        <v>0.99</v>
+      </c>
+      <c r="T41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="Q42" t="s">
+        <v>12</v>
+      </c>
+      <c r="R42" t="s">
+        <v>5</v>
+      </c>
+      <c r="S42">
+        <v>0.99</v>
+      </c>
+      <c r="T42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="Q43" t="s">
+        <v>12</v>
+      </c>
+      <c r="R43" t="s">
+        <v>5</v>
+      </c>
+      <c r="S43">
+        <v>0.99</v>
+      </c>
+      <c r="T43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="Q44" t="s">
+        <v>12</v>
+      </c>
+      <c r="R44" t="s">
+        <v>5</v>
+      </c>
+      <c r="S44">
+        <v>0.99</v>
+      </c>
+      <c r="T44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="Q45" t="s">
+        <v>12</v>
+      </c>
+      <c r="R45" t="s">
+        <v>18</v>
+      </c>
+      <c r="S45">
+        <v>0.6</v>
+      </c>
+      <c r="T45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="Q46" t="s">
+        <v>12</v>
+      </c>
+      <c r="R46" t="s">
+        <v>18</v>
+      </c>
+      <c r="S46">
+        <v>0.15</v>
+      </c>
+      <c r="T46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="Q47" t="s">
+        <v>12</v>
+      </c>
+      <c r="R47" t="s">
+        <v>18</v>
+      </c>
+      <c r="S47">
+        <v>0.11</v>
+      </c>
+      <c r="T47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="Q48" t="s">
+        <v>12</v>
+      </c>
+      <c r="R48" t="s">
+        <v>18</v>
+      </c>
+      <c r="S48">
+        <v>0.08</v>
+      </c>
+      <c r="T48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q49" t="s">
+        <v>12</v>
+      </c>
+      <c r="R49" t="s">
+        <v>18</v>
+      </c>
+      <c r="S49">
+        <v>0.05</v>
+      </c>
+      <c r="T49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q50" t="s">
+        <v>12</v>
+      </c>
+      <c r="R50" t="s">
+        <v>19</v>
+      </c>
+      <c r="S50">
+        <v>23.2</v>
+      </c>
+      <c r="T50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q51" t="s">
+        <v>12</v>
+      </c>
+      <c r="R51" t="s">
+        <v>19</v>
+      </c>
+      <c r="S51">
+        <v>5.7</v>
+      </c>
+      <c r="T51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q52" t="s">
+        <v>12</v>
+      </c>
+      <c r="R52" t="s">
+        <v>19</v>
+      </c>
+      <c r="S52">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="T52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q53" t="s">
+        <v>12</v>
+      </c>
+      <c r="R53" t="s">
+        <v>19</v>
+      </c>
+      <c r="S53">
+        <v>3</v>
+      </c>
+      <c r="T53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q54" t="s">
+        <v>12</v>
+      </c>
+      <c r="R54" t="s">
+        <v>19</v>
+      </c>
+      <c r="S54">
+        <v>2</v>
+      </c>
+      <c r="T54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q55" t="s">
+        <v>12</v>
+      </c>
+      <c r="R55" t="s">
+        <v>20</v>
+      </c>
+      <c r="S55">
+        <v>1</v>
+      </c>
+      <c r="T55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q56" t="s">
+        <v>12</v>
+      </c>
+      <c r="R56" t="s">
+        <v>20</v>
+      </c>
+      <c r="S56">
+        <v>3.4</v>
+      </c>
+      <c r="T56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q57" t="s">
+        <v>12</v>
+      </c>
+      <c r="R57" t="s">
+        <v>20</v>
+      </c>
+      <c r="S57">
+        <v>3.03</v>
+      </c>
+      <c r="T57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q58" t="s">
+        <v>12</v>
+      </c>
+      <c r="R58" t="s">
+        <v>20</v>
+      </c>
+      <c r="S58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q59" t="s">
+        <v>12</v>
+      </c>
+      <c r="R59" t="s">
+        <v>20</v>
+      </c>
+      <c r="S59">
+        <v>1.3</v>
+      </c>
+      <c r="T59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q60" t="s">
+        <v>22</v>
+      </c>
+      <c r="R60" t="s">
+        <v>5</v>
+      </c>
+      <c r="S60">
+        <v>1.31</v>
+      </c>
+      <c r="T60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q61" t="s">
+        <v>22</v>
+      </c>
+      <c r="R61" t="s">
+        <v>5</v>
+      </c>
+      <c r="S61">
+        <v>1.31</v>
+      </c>
+      <c r="T61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q62" t="s">
+        <v>22</v>
+      </c>
+      <c r="R62" t="s">
+        <v>5</v>
+      </c>
+      <c r="S62">
+        <v>1.31</v>
+      </c>
+      <c r="T62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q63" t="s">
+        <v>22</v>
+      </c>
+      <c r="R63" t="s">
+        <v>5</v>
+      </c>
+      <c r="S63">
+        <v>1.31</v>
+      </c>
+      <c r="T63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q64" t="s">
+        <v>22</v>
+      </c>
+      <c r="R64" t="s">
+        <v>5</v>
+      </c>
+      <c r="S64">
+        <v>1.31</v>
+      </c>
+      <c r="T64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q65" t="s">
+        <v>22</v>
+      </c>
+      <c r="R65" t="s">
+        <v>18</v>
+      </c>
+      <c r="S65">
+        <v>0.59</v>
+      </c>
+      <c r="T65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q66" t="s">
+        <v>22</v>
+      </c>
+      <c r="R66" t="s">
+        <v>18</v>
+      </c>
+      <c r="S66">
+        <v>0.21</v>
+      </c>
+      <c r="T66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q67" t="s">
+        <v>22</v>
+      </c>
+      <c r="R67" t="s">
+        <v>18</v>
+      </c>
+      <c r="S67">
+        <v>0.11</v>
+      </c>
+      <c r="T67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q68" t="s">
+        <v>22</v>
+      </c>
+      <c r="R68" t="s">
+        <v>18</v>
+      </c>
+      <c r="S68">
+        <v>0.06</v>
+      </c>
+      <c r="T68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q69" t="s">
+        <v>22</v>
+      </c>
+      <c r="R69" t="s">
+        <v>18</v>
+      </c>
+      <c r="S69">
+        <v>0.03</v>
+      </c>
+      <c r="T69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q70" t="s">
+        <v>22</v>
+      </c>
+      <c r="R70" t="s">
+        <v>19</v>
+      </c>
+      <c r="S70">
+        <v>22.1</v>
+      </c>
+      <c r="T70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q71" t="s">
+        <v>22</v>
+      </c>
+      <c r="R71" t="s">
+        <v>19</v>
+      </c>
+      <c r="S71">
+        <v>7.5</v>
+      </c>
+      <c r="T71">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q72" t="s">
+        <v>22</v>
+      </c>
+      <c r="R72" t="s">
+        <v>19</v>
+      </c>
+      <c r="S72">
+        <v>4.2</v>
+      </c>
+      <c r="T72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q73" t="s">
+        <v>22</v>
+      </c>
+      <c r="R73" t="s">
+        <v>19</v>
+      </c>
+      <c r="S73">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T73">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q74" t="s">
+        <v>22</v>
+      </c>
+      <c r="R74" t="s">
+        <v>19</v>
+      </c>
+      <c r="S74">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q75" t="s">
+        <v>22</v>
+      </c>
+      <c r="R75" t="s">
+        <v>20</v>
+      </c>
+      <c r="S75">
+        <v>1</v>
+      </c>
+      <c r="T75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q76" t="s">
+        <v>22</v>
+      </c>
+      <c r="R76" t="s">
+        <v>20</v>
+      </c>
+      <c r="S76">
+        <v>1.7</v>
+      </c>
+      <c r="T76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q77" t="s">
+        <v>22</v>
+      </c>
+      <c r="R77" t="s">
+        <v>20</v>
+      </c>
+      <c r="S77">
+        <v>1.7</v>
+      </c>
+      <c r="T77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q78" t="s">
+        <v>22</v>
+      </c>
+      <c r="R78" t="s">
+        <v>20</v>
+      </c>
+      <c r="S78">
+        <v>1.3</v>
+      </c>
+      <c r="T78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q79" t="s">
+        <v>22</v>
+      </c>
+      <c r="R79" t="s">
+        <v>20</v>
+      </c>
+      <c r="S79">
+        <v>0.48</v>
+      </c>
+      <c r="T79">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q80" t="s">
+        <v>23</v>
+      </c>
+      <c r="R80" t="s">
+        <v>5</v>
+      </c>
+      <c r="S80">
+        <v>0.623</v>
+      </c>
+      <c r="T80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q81" t="s">
+        <v>23</v>
+      </c>
+      <c r="R81" t="s">
+        <v>5</v>
+      </c>
+      <c r="S81">
+        <v>0.623</v>
+      </c>
+      <c r="T81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q82" t="s">
+        <v>23</v>
+      </c>
+      <c r="R82" t="s">
+        <v>5</v>
+      </c>
+      <c r="S82">
+        <v>0.623</v>
+      </c>
+      <c r="T82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q83" t="s">
+        <v>23</v>
+      </c>
+      <c r="R83" t="s">
+        <v>5</v>
+      </c>
+      <c r="S83">
+        <v>0.623</v>
+      </c>
+      <c r="T83">
+        <v>4</v>
+      </c>
+      <c r="W83" t="s">
+        <v>21</v>
+      </c>
+      <c r="X83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q84" t="s">
+        <v>23</v>
+      </c>
+      <c r="R84" t="s">
+        <v>5</v>
+      </c>
+      <c r="S84">
+        <v>0.623</v>
+      </c>
+      <c r="T84">
+        <v>5</v>
+      </c>
+      <c r="W84" t="s">
+        <v>4</v>
+      </c>
+      <c r="X84">
+        <v>0.623</v>
+      </c>
+    </row>
+    <row r="85" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q85" t="s">
+        <v>23</v>
+      </c>
+      <c r="R85" t="s">
+        <v>18</v>
+      </c>
+      <c r="S85">
+        <v>0.17</v>
+      </c>
+      <c r="T85">
+        <v>1</v>
+      </c>
+      <c r="W85" t="s">
+        <v>3</v>
+      </c>
+      <c r="X85">
+        <v>1</v>
+      </c>
+      <c r="Y85">
+        <v>2</v>
+      </c>
+      <c r="Z85">
+        <v>3</v>
+      </c>
+      <c r="AA85">
+        <v>4</v>
+      </c>
+      <c r="AB85">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q86" t="s">
+        <v>23</v>
+      </c>
+      <c r="R86" t="s">
+        <v>18</v>
+      </c>
+      <c r="S86">
+        <v>0.15</v>
+      </c>
+      <c r="T86">
+        <v>2</v>
+      </c>
+      <c r="W86" t="s">
+        <v>0</v>
+      </c>
+      <c r="X86">
+        <v>0.17</v>
+      </c>
+      <c r="Y86">
+        <v>0.15</v>
+      </c>
+      <c r="Z86">
+        <v>0.19</v>
+      </c>
+      <c r="AA86">
+        <v>0.23</v>
+      </c>
+      <c r="AB86">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="87" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q87" t="s">
+        <v>23</v>
+      </c>
+      <c r="R87" t="s">
+        <v>18</v>
+      </c>
+      <c r="S87">
+        <v>0.19</v>
+      </c>
+      <c r="T87">
+        <v>3</v>
+      </c>
+      <c r="W87" t="s">
+        <v>1</v>
+      </c>
+      <c r="X87">
+        <v>5.2</v>
+      </c>
+      <c r="Y87">
+        <v>4.8</v>
+      </c>
+      <c r="Z87">
+        <v>5.9</v>
+      </c>
+      <c r="AA87">
+        <v>6.4</v>
+      </c>
+      <c r="AB87">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="88" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q88" t="s">
+        <v>23</v>
+      </c>
+      <c r="R88" t="s">
+        <v>18</v>
+      </c>
+      <c r="S88">
+        <v>0.23</v>
+      </c>
+      <c r="T88">
+        <v>4</v>
+      </c>
+      <c r="W88" t="s">
+        <v>2</v>
+      </c>
+      <c r="X88">
+        <v>1</v>
+      </c>
+      <c r="Y88">
+        <v>1.4</v>
+      </c>
+      <c r="Z88">
+        <v>0.8</v>
+      </c>
+      <c r="AA88">
+        <v>0.46</v>
+      </c>
+      <c r="AB88">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="89" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q89" t="s">
+        <v>23</v>
+      </c>
+      <c r="R89" t="s">
+        <v>18</v>
+      </c>
+      <c r="S89">
+        <v>0.26</v>
+      </c>
+      <c r="T89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q90" t="s">
+        <v>23</v>
+      </c>
+      <c r="R90" t="s">
+        <v>19</v>
+      </c>
+      <c r="S90">
+        <v>5.2</v>
+      </c>
+      <c r="T90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q91" t="s">
+        <v>23</v>
+      </c>
+      <c r="R91" t="s">
+        <v>19</v>
+      </c>
+      <c r="S91">
+        <v>4.8</v>
+      </c>
+      <c r="T91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q92" t="s">
+        <v>23</v>
+      </c>
+      <c r="R92" t="s">
+        <v>19</v>
+      </c>
+      <c r="S92">
+        <v>5.9</v>
+      </c>
+      <c r="T92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q93" t="s">
+        <v>23</v>
+      </c>
+      <c r="R93" t="s">
+        <v>19</v>
+      </c>
+      <c r="S93">
+        <v>6.4</v>
+      </c>
+      <c r="T93">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q94" t="s">
+        <v>23</v>
+      </c>
+      <c r="R94" t="s">
+        <v>19</v>
+      </c>
+      <c r="S94">
+        <v>6.7</v>
+      </c>
+      <c r="T94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q95" t="s">
+        <v>23</v>
+      </c>
+      <c r="R95" t="s">
+        <v>20</v>
+      </c>
+      <c r="S95">
+        <v>1</v>
+      </c>
+      <c r="T95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="17:28" x14ac:dyDescent="0.2">
+      <c r="Q96" t="s">
+        <v>23</v>
+      </c>
+      <c r="R96" t="s">
+        <v>20</v>
+      </c>
+      <c r="S96">
+        <v>1.4</v>
+      </c>
+      <c r="T96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q97" t="s">
+        <v>23</v>
+      </c>
+      <c r="R97" t="s">
+        <v>20</v>
+      </c>
+      <c r="S97">
+        <v>0.8</v>
+      </c>
+      <c r="T97">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q98" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R98" t="s">
+        <v>20</v>
+      </c>
+      <c r="S98">
+        <v>0.46</v>
+      </c>
+      <c r="T98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="17:20" x14ac:dyDescent="0.2">
+      <c r="Q99" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R99" t="s">
+        <v>20</v>
+      </c>
+      <c r="S99">
+        <v>0.21</v>
+      </c>
+      <c r="T99">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1841,23 +2786,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B611C603-668F-6F4B-8C20-77C3DED97A8F}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1865,7 +2810,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -1879,7 +2824,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -1893,7 +2838,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -1907,7 +2852,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1921,7 +2866,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1935,10 +2880,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>0.6</v>
@@ -1949,10 +2894,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>0.2</v>
@@ -1963,10 +2908,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>0.1</v>
@@ -1977,10 +2922,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>0.06</v>
@@ -1991,10 +2936,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11">
         <v>0.03</v>
@@ -2005,10 +2950,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>21.3</v>
@@ -2019,10 +2964,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13">
         <v>7.3</v>
@@ -2033,10 +2978,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14">
         <v>4</v>
@@ -2047,10 +2992,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>2.1</v>
@@ -2061,10 +3006,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16">
         <v>1.1000000000000001</v>
@@ -2075,10 +3020,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2089,10 +3034,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C18">
         <v>1.7</v>
@@ -2103,10 +3048,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>1.8</v>
@@ -2117,10 +3062,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>1.5</v>
@@ -2131,15 +3076,855 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C21">
         <v>0.96</v>
       </c>
       <c r="D21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <v>0.99</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>0.99</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <v>0.99</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25">
+        <v>0.99</v>
+      </c>
+      <c r="D25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>0.99</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>0.6</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28">
+        <v>0.15</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29">
+        <v>0.11</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30">
+        <v>0.08</v>
+      </c>
+      <c r="D30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <v>0.05</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32">
+        <v>23.2</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33">
+        <v>5.7</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" t="s">
+        <v>20</v>
+      </c>
+      <c r="C38">
+        <v>3.4</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <v>3.03</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41">
+        <v>1.3</v>
+      </c>
+      <c r="D41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>1.31</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>1.31</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>1.31</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>1.31</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>1.31</v>
+      </c>
+      <c r="D46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47">
+        <v>0.59</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+      <c r="C48">
+        <v>0.21</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C49">
+        <v>0.11</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50">
+        <v>0.06</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51">
+        <v>0.03</v>
+      </c>
+      <c r="D51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52">
+        <v>22.1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53">
+        <v>7.5</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54">
+        <v>4.2</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" t="s">
+        <v>20</v>
+      </c>
+      <c r="C58">
+        <v>1.7</v>
+      </c>
+      <c r="D58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59">
+        <v>1.7</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60">
+        <v>1.3</v>
+      </c>
+      <c r="D60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>22</v>
+      </c>
+      <c r="B61" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61">
+        <v>0.48</v>
+      </c>
+      <c r="D61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62">
+        <v>0.623</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63">
+        <v>0.623</v>
+      </c>
+      <c r="D63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64">
+        <v>0.623</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65">
+        <v>0.623</v>
+      </c>
+      <c r="D65">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66">
+        <v>0.623</v>
+      </c>
+      <c r="D66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" t="s">
+        <v>18</v>
+      </c>
+      <c r="C67">
+        <v>0.17</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C68">
+        <v>0.15</v>
+      </c>
+      <c r="D68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" t="s">
+        <v>18</v>
+      </c>
+      <c r="C69">
+        <v>0.19</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70">
+        <v>0.23</v>
+      </c>
+      <c r="D70">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" t="s">
+        <v>18</v>
+      </c>
+      <c r="C71">
+        <v>0.26</v>
+      </c>
+      <c r="D71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72">
+        <v>5.2</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73">
+        <v>4.8</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" t="s">
+        <v>19</v>
+      </c>
+      <c r="C74">
+        <v>5.9</v>
+      </c>
+      <c r="D74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" t="s">
+        <v>19</v>
+      </c>
+      <c r="C75">
+        <v>6.4</v>
+      </c>
+      <c r="D75">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C76">
+        <v>6.7</v>
+      </c>
+      <c r="D76">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>23</v>
+      </c>
+      <c r="B77" t="s">
+        <v>20</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>23</v>
+      </c>
+      <c r="B78" t="s">
+        <v>20</v>
+      </c>
+      <c r="C78">
+        <v>1.4</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>23</v>
+      </c>
+      <c r="B79" t="s">
+        <v>20</v>
+      </c>
+      <c r="C79">
+        <v>0.8</v>
+      </c>
+      <c r="D79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80" t="s">
+        <v>20</v>
+      </c>
+      <c r="C80">
+        <v>0.46</v>
+      </c>
+      <c r="D80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B81" t="s">
+        <v>20</v>
+      </c>
+      <c r="C81">
+        <v>0.21</v>
+      </c>
+      <c r="D81">
         <v>5</v>
       </c>
     </row>

</xml_diff>